<commit_message>
Pripremljeni svi testovi , pojedinacno webperformance testovi provereni i rade kako treba , u nekim slucajevima
</commit_message>
<xml_diff>
--- a/Lista testova za Regression test (Autosaved).xlsx
+++ b/Lista testova za Regression test (Autosaved).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="143">
   <si>
     <t>LISTA TESTOVA ZA REGRESSION TEST</t>
   </si>
@@ -373,9 +373,6 @@
     <t>Submission Detail page</t>
   </si>
   <si>
-    <t>SubmissionDetail</t>
-  </si>
-  <si>
     <t>File Action - Edit</t>
   </si>
   <si>
@@ -571,6 +568,9 @@
 4. Global submission list
 5. Pronalazenje submissiona i otvaranje
 6. Provera da li su podaci identicni spremljenim tokom publish-ovanja </t>
+  </si>
+  <si>
+    <t>SubmissionDetail LLMR04</t>
   </si>
 </sst>
 </file>
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1204,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1221,7 +1221,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1235,10 +1235,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1252,10 +1252,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1272,7 +1272,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1289,7 +1289,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1306,7 +1306,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1323,7 +1323,7 @@
         <v>22</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1334,13 +1334,13 @@
         <v>23</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1357,7 +1357,7 @@
         <v>26</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1368,129 +1368,129 @@
         <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="22"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>125</v>
-      </c>
       <c r="E21" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>127</v>
-      </c>
       <c r="E22" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -1501,13 +1501,13 @@
         <v>29</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1518,13 +1518,13 @@
         <v>31</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1541,7 +1541,7 @@
         <v>35</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1558,7 +1558,7 @@
         <v>38</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1569,13 +1569,13 @@
         <v>39</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1592,7 +1592,7 @@
         <v>45</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1609,7 +1609,7 @@
         <v>46</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1626,7 +1626,7 @@
         <v>47</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1643,7 +1643,7 @@
         <v>48</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
         <v>69</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1677,7 +1677,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
         <v>71</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1711,7 +1711,7 @@
         <v>72</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1728,7 +1728,7 @@
         <v>73</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1745,7 +1745,7 @@
         <v>74</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1762,7 +1762,7 @@
         <v>75</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1779,7 +1779,7 @@
         <v>76</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1790,13 +1790,13 @@
         <v>77</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>78</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="165" x14ac:dyDescent="0.25">
@@ -1807,55 +1807,61 @@
         <v>79</v>
       </c>
       <c r="C41" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E41" s="22"/>
+      <c r="E41" s="22" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>30</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E42" s="22"/>
+        <v>97</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>31</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E43" s="22"/>
+        <v>98</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>32</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E44" s="22"/>
     </row>
@@ -1864,13 +1870,13 @@
         <v>33</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E45" s="22"/>
     </row>
@@ -1879,13 +1885,13 @@
         <v>34</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E46" s="22"/>
     </row>
@@ -1894,13 +1900,13 @@
         <v>35</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E47" s="22"/>
     </row>
@@ -1909,16 +1915,16 @@
         <v>36</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1926,13 +1932,13 @@
         <v>37</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E49" s="23"/>
     </row>

</xml_diff>

<commit_message>
Kreian Load test sa nazivom REGRESSION TEST u kojem se nalazi svih 36 pojedinacnih testova. Pusten, pojavilo se nekoliko gresaka, prouzrokovane pre svega time sto nije izvrsen postupak slanja u win service ( ranije isao na 3 minute a sada na 30 minuta ).  Ostale greske ne javljaju se kada se testovi pustaju pojedinacno. Ovde zaustavljamo prvu verziju i pravimo novi branch u slucaju da se nastavi sa razvojem.
</commit_message>
<xml_diff>
--- a/Lista testova za Regression test (Autosaved).xlsx
+++ b/Lista testova za Regression test (Autosaved).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="140">
   <si>
     <t>LISTA TESTOVA ZA REGRESSION TEST</t>
   </si>
@@ -385,9 +385,6 @@
     <t>File Action - Cancel</t>
   </si>
   <si>
-    <t>Submission Detail page - Submitted Data</t>
-  </si>
-  <si>
     <t>Submission Detail page - Submission History</t>
   </si>
   <si>
@@ -406,9 +403,6 @@
     <t>Obrisati jedan postojeci submission I proveriti da li se javlja na MyDashboard stranici I na Global submission Listi</t>
   </si>
   <si>
-    <t>Kreirati novi submission I proveriti da li se isti podaci pojavljuju I na Submitted Data prikazu</t>
-  </si>
-  <si>
     <t>Kreirati submission I poslati ga do CH a zatim pogledati da li je History popunjen ispravno</t>
   </si>
   <si>
@@ -428,9 +422,6 @@
   </si>
   <si>
     <t>FileActionExporttoPDF</t>
-  </si>
-  <si>
-    <t>SubmissionDetailpageSubmitted Data</t>
   </si>
   <si>
     <t>SubmissionDetailpageSubmission History</t>
@@ -1170,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E49"/>
+  <dimension ref="A2:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1195,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1221,7 +1212,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1235,10 +1226,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1252,10 +1243,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1272,7 +1263,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1289,7 +1280,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1306,7 +1297,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1323,7 +1314,7 @@
         <v>22</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1334,13 +1325,13 @@
         <v>23</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1357,7 +1348,7 @@
         <v>26</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1368,129 +1359,129 @@
         <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="22"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -1501,13 +1492,13 @@
         <v>29</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1518,13 +1509,13 @@
         <v>31</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1541,7 +1532,7 @@
         <v>35</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1558,7 +1549,7 @@
         <v>38</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1569,13 +1560,13 @@
         <v>39</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1592,7 +1583,7 @@
         <v>45</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1609,7 +1600,7 @@
         <v>46</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1626,7 +1617,7 @@
         <v>47</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1643,7 +1634,7 @@
         <v>48</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1660,7 +1651,7 @@
         <v>69</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1677,7 +1668,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1694,7 +1685,7 @@
         <v>71</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1711,7 +1702,7 @@
         <v>72</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1728,7 +1719,7 @@
         <v>73</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1745,7 +1736,7 @@
         <v>74</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1762,7 +1753,7 @@
         <v>75</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1779,7 +1770,7 @@
         <v>76</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1790,13 +1781,13 @@
         <v>77</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>78</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="165" x14ac:dyDescent="0.25">
@@ -1807,13 +1798,13 @@
         <v>79</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1824,13 +1815,13 @@
         <v>80</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1841,13 +1832,13 @@
         <v>81</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1858,12 +1849,14 @@
         <v>82</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E44" s="22"/>
+        <v>93</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
@@ -1873,12 +1866,14 @@
         <v>83</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E45" s="22"/>
+        <v>94</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
@@ -1888,14 +1883,16 @@
         <v>84</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E46" s="22"/>
-    </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>35</v>
       </c>
@@ -1903,44 +1900,29 @@
         <v>85</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E47" s="22"/>
-    </row>
-    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>36</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E48" s="22" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7">
-        <v>37</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E49" s="23"/>
+      <c r="C48" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>